<commit_message>
energy carrier tax rate and mark-up updates for historic and future scenario simulations. presentation of the RokiG JF of 03.06 is added.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_EnergyCarrier_Price_MarkUp.xlsx
+++ b/projects/test_building/input/Scenario_EnergyCarrier_Price_MarkUp.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D169227D-48E6-DB41-B0D2-BAF2EC3731C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-960" yWindow="-20220" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-960" yWindow="-20220" windowWidth="30240" windowHeight="17385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="note" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -184,7 +183,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -344,56 +343,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:AU25" totalsRowShown="0">
-  <autoFilter ref="A1:AU25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AU25" totalsRowShown="0">
+  <autoFilter ref="A1:AU25"/>
   <tableColumns count="47">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_scenario"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="id_region"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_sector"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_energy_carrier"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="unit"/>
-    <tableColumn id="40" xr3:uid="{5A259EF6-EFC7-AF47-A817-EBF89983F4FF}" name="2010"/>
-    <tableColumn id="41" xr3:uid="{2F1B74DF-194A-7C4B-8075-FB97ED14085F}" name="2011"/>
-    <tableColumn id="42" xr3:uid="{12FADAC8-A570-3A4A-A980-E9CA70E75444}" name="2012"/>
-    <tableColumn id="43" xr3:uid="{DD76AF02-8F31-494B-A06E-FFA71EB64DE1}" name="2013"/>
-    <tableColumn id="44" xr3:uid="{1B09AE6F-1AB9-5443-8A15-399F2A544996}" name="2014"/>
-    <tableColumn id="45" xr3:uid="{B2CA028C-EA02-C34F-8B32-ED11DE1159DE}" name="2015"/>
-    <tableColumn id="46" xr3:uid="{279EC927-AC6F-4448-8AA4-BFE44A2299F9}" name="2016"/>
-    <tableColumn id="47" xr3:uid="{6069D95F-5B77-FC4F-BBD3-F8342C38999E}" name="2017"/>
-    <tableColumn id="48" xr3:uid="{07A26060-5D13-AC4D-BDAD-5D5E6EA69DF3}" name="2018"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="2019" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2020" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2021" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2022" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="2023" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2024" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="2025" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="2026" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="2027" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="2028" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="2029" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="2030" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="2031" dataDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="2032" dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="2033" dataDxfId="18"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="2034" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="2035" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="2036" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="2037" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="2038" dataDxfId="13"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="2039" dataDxfId="12"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="2040" dataDxfId="11"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="2041" dataDxfId="10"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="2042" dataDxfId="9"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="2043" dataDxfId="8"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="2044" dataDxfId="7"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="2045" dataDxfId="6"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="2046" dataDxfId="5"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="2047" dataDxfId="4"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="2048" dataDxfId="3"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="2049" dataDxfId="2"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="2050" dataDxfId="1"/>
-    <tableColumn id="38" xr3:uid="{60E71B52-D41B-5943-8E9D-156570FE78A9}" name="2051" dataDxfId="0"/>
+    <tableColumn id="1" name="id_scenario"/>
+    <tableColumn id="2" name="id_region"/>
+    <tableColumn id="3" name="id_sector"/>
+    <tableColumn id="4" name="id_energy_carrier"/>
+    <tableColumn id="5" name="unit"/>
+    <tableColumn id="40" name="2010"/>
+    <tableColumn id="41" name="2011"/>
+    <tableColumn id="42" name="2012"/>
+    <tableColumn id="43" name="2013"/>
+    <tableColumn id="44" name="2014"/>
+    <tableColumn id="45" name="2015"/>
+    <tableColumn id="46" name="2016"/>
+    <tableColumn id="47" name="2017"/>
+    <tableColumn id="48" name="2018"/>
+    <tableColumn id="6" name="2019" dataDxfId="32"/>
+    <tableColumn id="7" name="2020" dataDxfId="31"/>
+    <tableColumn id="8" name="2021" dataDxfId="30"/>
+    <tableColumn id="9" name="2022" dataDxfId="29"/>
+    <tableColumn id="10" name="2023" dataDxfId="28"/>
+    <tableColumn id="11" name="2024" dataDxfId="27"/>
+    <tableColumn id="12" name="2025" dataDxfId="26"/>
+    <tableColumn id="13" name="2026" dataDxfId="25"/>
+    <tableColumn id="14" name="2027" dataDxfId="24"/>
+    <tableColumn id="15" name="2028" dataDxfId="23"/>
+    <tableColumn id="16" name="2029" dataDxfId="22"/>
+    <tableColumn id="17" name="2030" dataDxfId="21"/>
+    <tableColumn id="18" name="2031" dataDxfId="20"/>
+    <tableColumn id="19" name="2032" dataDxfId="19"/>
+    <tableColumn id="20" name="2033" dataDxfId="18"/>
+    <tableColumn id="21" name="2034" dataDxfId="17"/>
+    <tableColumn id="22" name="2035" dataDxfId="16"/>
+    <tableColumn id="23" name="2036" dataDxfId="15"/>
+    <tableColumn id="24" name="2037" dataDxfId="14"/>
+    <tableColumn id="25" name="2038" dataDxfId="13"/>
+    <tableColumn id="26" name="2039" dataDxfId="12"/>
+    <tableColumn id="27" name="2040" dataDxfId="11"/>
+    <tableColumn id="28" name="2041" dataDxfId="10"/>
+    <tableColumn id="29" name="2042" dataDxfId="9"/>
+    <tableColumn id="30" name="2043" dataDxfId="8"/>
+    <tableColumn id="31" name="2044" dataDxfId="7"/>
+    <tableColumn id="32" name="2045" dataDxfId="6"/>
+    <tableColumn id="33" name="2046" dataDxfId="5"/>
+    <tableColumn id="34" name="2047" dataDxfId="4"/>
+    <tableColumn id="35" name="2048" dataDxfId="3"/>
+    <tableColumn id="36" name="2049" dataDxfId="2"/>
+    <tableColumn id="37" name="2050" dataDxfId="1"/>
+    <tableColumn id="38" name="2051" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -661,24 +660,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="AT13" sqref="AT13"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -821,7 +820,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -838,133 +837,133 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>2.4699999999999993E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>3.500000000000001E-2</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>4.1349999999999998E-2</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>5.7849999999999999E-2</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>7.1849999999999997E-2</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>7.4899999999999994E-2</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>7.85E-2</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>8.7650000000000006E-2</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>0.10005000000000001</v>
       </c>
       <c r="R2" s="1">
-        <v>0</v>
+        <v>5.510000000000001E-2</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>3.5299999999999984E-2</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="U2" s="1">
-        <v>0</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="V2" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="Y2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AA2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AB2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AC2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AD2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AE2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AF2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AG2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AH2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AK2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AL2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AM2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AN2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AO2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AP2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AQ2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AR2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AS2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AT2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AU2" s="1">
-        <v>0</v>
+        <v>5.5E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1267,133 +1266,133 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>4.9499999999999995E-3</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>4.9499999999999995E-3</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>4.0500000000000015E-3</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>4.0500000000000015E-3</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>4.0500000000000015E-3</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>3.9999999999999966E-3</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>4.049999999999998E-3</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>4.049999999999998E-3</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>4.0999999999999995E-3</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>5.0499999999999955E-3</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>6.0000000000000019E-3</v>
       </c>
       <c r="Q5" s="1">
-        <v>0</v>
+        <v>1.0199999999999997E-2</v>
       </c>
       <c r="R5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>1.575E-2</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="U5" s="1">
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="V5" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="W5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="X5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="Y5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="Z5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AA5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AB5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AC5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AD5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AE5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AF5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AG5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AH5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AK5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AL5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AM5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AN5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AO5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AP5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AQ5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AR5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AS5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AT5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
       <c r="AU5" s="1">
-        <v>0</v>
+        <v>1.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2554,133 +2553,133 @@
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>6.4699999999999994E-2</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>7.2499999999999995E-2</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>7.7849999999999989E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>9.6299999999999997E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>0.10645000000000002</v>
       </c>
       <c r="K14" s="1">
-        <v>0</v>
+        <v>0.10489999999999999</v>
       </c>
       <c r="L14" s="1">
-        <v>0</v>
+        <v>0.11134999999999999</v>
       </c>
       <c r="M14" s="1">
-        <v>0</v>
+        <v>0.11749999999999999</v>
       </c>
       <c r="N14" s="1">
-        <v>0</v>
+        <v>0.1137</v>
       </c>
       <c r="O14" s="1">
-        <v>0</v>
+        <v>0.11095000000000001</v>
       </c>
       <c r="P14" s="1">
-        <v>0</v>
+        <v>0.11370000000000001</v>
       </c>
       <c r="Q14" s="1">
-        <v>0</v>
+        <v>0.11220000000000001</v>
       </c>
       <c r="R14" s="1">
-        <v>0</v>
+        <v>6.7299999999999999E-2</v>
       </c>
       <c r="S14" s="1">
-        <v>0</v>
+        <v>4.9549999999999983E-2</v>
       </c>
       <c r="T14" s="1">
-        <v>0</v>
+        <v>5.5550000000000002E-2</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="V14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="W14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="X14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="Y14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="Z14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AA14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AB14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AC14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AD14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AE14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AF14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AG14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AH14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AI14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AJ14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AK14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AL14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AM14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AN14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AO14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AP14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AQ14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AR14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AS14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AT14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="AU14" s="1">
-        <v>0</v>
+        <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2966,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2983,133 +2982,133 @@
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>5.9999999999999984E-3</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>5.899999999999999E-3</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>5.899999999999999E-3</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>5.9500000000000004E-3</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>6.0000000000000019E-3</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>5.9500000000000004E-3</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>5.9500000000000004E-3</v>
       </c>
       <c r="M17" s="1">
-        <v>0</v>
+        <v>5.9500000000000004E-3</v>
       </c>
       <c r="N17" s="1">
-        <v>0</v>
+        <v>5.9500000000000004E-3</v>
       </c>
       <c r="O17" s="1">
-        <v>0</v>
+        <v>6.1000000000000013E-3</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>6.3E-3</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>1.0800000000000004E-2</v>
       </c>
       <c r="R17" s="1">
-        <v>0</v>
+        <v>1.1799999999999998E-2</v>
       </c>
       <c r="S17" s="1">
-        <v>0</v>
+        <v>1.6E-2</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="U17" s="1">
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="V17" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="W17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="X17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="Y17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="Z17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AA17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AB17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AC17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AD17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AE17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AF17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AG17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AH17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AI17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AJ17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AK17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AL17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AM17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AN17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AO17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AP17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AQ17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AR17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AS17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AT17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AU17" s="1">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3252,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -3395,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -3538,7 +3537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3824,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3967,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -4263,14 +4262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FABCDCF-667B-9243-ADF9-4D8A4917B735}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>

</xml_diff>